<commit_message>
add design and cost of pit latrine
</commit_message>
<xml_diff>
--- a/sanitation/systems/bwaise/inputs/defaults.xlsx
+++ b/sanitation/systems/bwaise/inputs/defaults.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/systems/bwaise/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B26365CA-7E27-C44A-9972-5BCA5A4FEFB3}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77E5E344-30CD-2D45-AC8C-993C00D25544}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="3240" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
+    <workbookView xWindow="10760" yWindow="3340" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
   </bookViews>
   <sheets>
-    <sheet name="excretion" sheetId="1" r:id="rId1"/>
-    <sheet name="user_interface" sheetId="2" r:id="rId2"/>
+    <sheet name="Excretion" sheetId="1" r:id="rId1"/>
+    <sheet name="PitLatrine" sheetId="2" r:id="rId2"/>
+    <sheet name="GHG-CFs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
   <si>
     <t>caloric_intake</t>
   </si>
@@ -327,6 +328,48 @@
   </si>
   <si>
     <t>N_fec_NH3</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>kg CO2eq/kg</t>
+  </si>
+  <si>
+    <t>kg CO2eq/m3</t>
+  </si>
+  <si>
+    <t>ecoinvent 3</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Stainless steel sheet</t>
+  </si>
+  <si>
+    <t>Stainless steel</t>
+  </si>
+  <si>
+    <t>Excavation</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Gravel</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>Bricks</t>
+  </si>
+  <si>
+    <t>Wood</t>
   </si>
 </sst>
 </file>
@@ -336,7 +379,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,8 +415,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +434,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -400,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -408,6 +464,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7BC447-558C-1948-86CA-9891C0EAE965}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1436,4 +1497,279 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C2D264-D2FC-E145-8DD9-6E517EFDD164}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.13</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.33</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.07</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.97</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.93</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.08</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1.19</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="2">
+        <v>197</v>
+      </c>
+      <c r="D11" s="2">
+        <v>186</v>
+      </c>
+      <c r="E11" s="2">
+        <v>208</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>